<commit_message>
added code for bridge
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D86A822-7EE7-40FD-A9C0-6164790C704F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD70DEE-7F3A-4CAC-9119-38A1FE5141DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="497">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1495,6 +1495,36 @@
   </si>
   <si>
     <t>run a triple for loop, first for the elemtnt k, find I and j such that matrix[i][j] &gt; matrix[i][k]+matrix[k][j] as the node k should be connected with all three</t>
+  </si>
+  <si>
+    <t>BFS, use a queue to store the positions and make a vector of boolean values to check if any node is revisited. For each q element, run a loop for 6 dice rools, and add if to the list if they are not visited already. Get the next row and coloum using maths in the next cell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  int get(int s,int n){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int quot=(s-1)/n;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int rem=(s-1)%n;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int row=n-quot-1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int col=row%2!=(n%2) ? rem : n-1-rem;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return row*n+col;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t>Perform dpf for the graph, maintain the parent array for each node, also make two arrays one for counting the number of time any node is seen and one for finding the lowest parent. If any point low[v]&lt;dis[v] you have a bridge</t>
+  </si>
+  <si>
+    <t>same as belman ford</t>
   </si>
 </sst>
 </file>
@@ -1627,21 +1657,21 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1955,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D481"/>
+  <dimension ref="A1:AC481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B364" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F381" sqref="F381"/>
+    <sheetView tabSelected="1" topLeftCell="A358" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G390" sqref="G390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5849,7 +5879,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="369" spans="1:4" ht="21">
+    <row r="369" spans="1:29" ht="21">
       <c r="A369" s="8" t="s">
         <v>343</v>
       </c>
@@ -5863,7 +5893,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="370" spans="1:4" ht="21">
+    <row r="370" spans="1:29" ht="21">
       <c r="A370" s="8" t="s">
         <v>343</v>
       </c>
@@ -5877,7 +5907,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="371" spans="1:4" ht="21">
+    <row r="371" spans="1:29" ht="21">
       <c r="A371" s="8" t="s">
         <v>343</v>
       </c>
@@ -5891,7 +5921,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="372" spans="1:4" ht="21">
+    <row r="372" spans="1:29" ht="21">
       <c r="A372" s="8" t="s">
         <v>343</v>
       </c>
@@ -5902,7 +5932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="373" spans="1:4" ht="21">
+    <row r="373" spans="1:29" ht="21">
       <c r="A373" s="8" t="s">
         <v>343</v>
       </c>
@@ -5913,7 +5943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="374" spans="1:4" ht="21">
+    <row r="374" spans="1:29" ht="21">
       <c r="A374" s="8" t="s">
         <v>343</v>
       </c>
@@ -5927,7 +5957,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="375" spans="1:4" ht="21">
+    <row r="375" spans="1:29" ht="21">
       <c r="A375" s="8" t="s">
         <v>343</v>
       </c>
@@ -5941,7 +5971,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="376" spans="1:4" ht="21">
+    <row r="376" spans="1:29" ht="21">
       <c r="A376" s="8" t="s">
         <v>343</v>
       </c>
@@ -5955,7 +5985,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="377" spans="1:4" ht="21">
+    <row r="377" spans="1:29" ht="21">
       <c r="A377" s="8" t="s">
         <v>343</v>
       </c>
@@ -5969,7 +5999,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="378" spans="1:4" ht="21">
+    <row r="378" spans="1:29" ht="21">
       <c r="A378" s="8" t="s">
         <v>343</v>
       </c>
@@ -5977,10 +6007,10 @@
         <v>366</v>
       </c>
       <c r="C378" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="379" spans="1:4" ht="21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="379" spans="1:29" ht="21">
       <c r="A379" s="8" t="s">
         <v>343</v>
       </c>
@@ -5988,10 +6018,10 @@
         <v>367</v>
       </c>
       <c r="C379" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="380" spans="1:4" ht="21">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="380" spans="1:29" ht="21">
       <c r="A380" s="8" t="s">
         <v>343</v>
       </c>
@@ -5999,10 +6029,16 @@
         <v>368</v>
       </c>
       <c r="C380" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="381" spans="1:4" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D380" t="s">
+        <v>487</v>
+      </c>
+      <c r="AC380" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="381" spans="1:29" ht="21">
       <c r="A381" s="8" t="s">
         <v>343</v>
       </c>
@@ -6010,10 +6046,16 @@
         <v>369</v>
       </c>
       <c r="C381" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="382" spans="1:4" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D381" t="s">
+        <v>495</v>
+      </c>
+      <c r="AC381" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="382" spans="1:29" ht="21">
       <c r="A382" s="8" t="s">
         <v>343</v>
       </c>
@@ -6023,8 +6065,11 @@
       <c r="C382" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="383" spans="1:4" ht="21">
+      <c r="AC382" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="383" spans="1:29" ht="21">
       <c r="A383" s="8" t="s">
         <v>343</v>
       </c>
@@ -6034,8 +6079,11 @@
       <c r="C383" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="384" spans="1:4" ht="21">
+      <c r="AC383" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="384" spans="1:29" ht="21">
       <c r="A384" s="8" t="s">
         <v>343</v>
       </c>
@@ -6043,10 +6091,16 @@
         <v>372</v>
       </c>
       <c r="C384" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="385" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D384" t="s">
+        <v>496</v>
+      </c>
+      <c r="AC384" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="385" spans="1:29" ht="21">
       <c r="A385" s="8" t="s">
         <v>343</v>
       </c>
@@ -6056,8 +6110,11 @@
       <c r="C385" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="386" spans="1:3" ht="21">
+      <c r="AC385" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="386" spans="1:29" ht="21">
       <c r="A386" s="8" t="s">
         <v>343</v>
       </c>
@@ -6067,8 +6124,11 @@
       <c r="C386" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="387" spans="1:3" ht="21">
+      <c r="AC386" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="387" spans="1:29" ht="21">
       <c r="A387" s="8" t="s">
         <v>343</v>
       </c>
@@ -6079,7 +6139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="388" spans="1:3" ht="21">
+    <row r="388" spans="1:29" ht="21">
       <c r="A388" s="8" t="s">
         <v>343</v>
       </c>
@@ -6090,7 +6150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="389" spans="1:3" ht="21">
+    <row r="389" spans="1:29" ht="21">
       <c r="A389" s="8" t="s">
         <v>343</v>
       </c>
@@ -6101,7 +6161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="390" spans="1:3" ht="21">
+    <row r="390" spans="1:29" ht="21">
       <c r="A390" s="8" t="s">
         <v>343</v>
       </c>
@@ -6112,7 +6172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="391" spans="1:3" ht="21">
+    <row r="391" spans="1:29" ht="21">
       <c r="A391" s="8" t="s">
         <v>343</v>
       </c>
@@ -6123,7 +6183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="392" spans="1:3" ht="21">
+    <row r="392" spans="1:29" ht="21">
       <c r="A392" s="8" t="s">
         <v>343</v>
       </c>
@@ -6134,7 +6194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="393" spans="1:3" ht="21">
+    <row r="393" spans="1:29" ht="21">
       <c r="A393" s="8" t="s">
         <v>343</v>
       </c>
@@ -6145,7 +6205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="394" spans="1:3" ht="21">
+    <row r="394" spans="1:29" ht="21">
       <c r="A394" s="8" t="s">
         <v>343</v>
       </c>
@@ -6156,7 +6216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="395" spans="1:3" ht="21">
+    <row r="395" spans="1:29" ht="21">
       <c r="A395" s="8" t="s">
         <v>343</v>
       </c>
@@ -6167,7 +6227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="396" spans="1:3" ht="21">
+    <row r="396" spans="1:29" ht="21">
       <c r="A396" s="8" t="s">
         <v>343</v>
       </c>
@@ -6178,7 +6238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="21">
+    <row r="397" spans="1:29" ht="21">
       <c r="A397" s="8" t="s">
         <v>343</v>
       </c>
@@ -6189,7 +6249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="398" spans="1:3" ht="21">
+    <row r="398" spans="1:29" ht="21">
       <c r="A398" s="8" t="s">
         <v>343</v>
       </c>
@@ -6200,7 +6260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:3" ht="21">
+    <row r="399" spans="1:29" ht="21">
       <c r="A399" s="8" t="s">
         <v>343</v>
       </c>
@@ -6211,7 +6271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:3" ht="21">
+    <row r="400" spans="1:29" ht="21">
       <c r="B400" s="7"/>
       <c r="C400" s="4"/>
     </row>
@@ -7074,11 +7134,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:C481">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",C6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",C6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",C6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
reverse to make path added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDBBA7B-A63D-439F-9CE3-517F5390AC54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD15CFF6-AE9F-483F-91FE-849D4F50784D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="11520" yWindow="12" windowWidth="11568" windowHeight="12348" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="501">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1554,6 +1554,9 @@
   </si>
   <si>
     <t>Traverse the graph with DFS, keep adding the current distance, if it reaches equal to or more than k, return true. If not found down one of the paths, backtrack by seeting the path bool back to false after dfs utl function is called.  If not found return false.</t>
+  </si>
+  <si>
+    <t>Make a array for storing the colors from 0 to V, initialize with 0. now make a recurive function, with v=0 as the starting index of the colors array. If v==V return true. Otherwise loop throught the colors array and at all points if it is safe to give that color to any node, recurively call the same function with v=v+1.. If at any point it returns false, back track by removing colors[v]=0. if v==m return true</t>
   </si>
 </sst>
 </file>
@@ -2017,8 +2020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:AF481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B395" sqref="B395"/>
+    <sheetView tabSelected="1" topLeftCell="A382" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B410" sqref="B410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6230,9 +6233,11 @@
         <v>379</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D392" s="12"/>
+        <v>465</v>
+      </c>
+      <c r="D392" s="12" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="393" spans="1:32" ht="21">
       <c r="A393" s="8" t="s">

</xml_diff>

<commit_message>
updated excel for explanation
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD15CFF6-AE9F-483F-91FE-849D4F50784D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB56AE0-1755-4CAB-A27D-4F8A84C4AC84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="12" windowWidth="11568" windowHeight="12348" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="502">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1557,6 +1557,9 @@
   </si>
   <si>
     <t>Make a array for storing the colors from 0 to V, initialize with 0. now make a recurive function, with v=0 as the starting index of the colors array. If v==V return true. Otherwise loop throught the colors array and at all points if it is safe to give that color to any node, recurively call the same function with v=v+1.. If at any point it returns false, back track by removing colors[v]=0. if v==m return true</t>
+  </si>
+  <si>
+    <t>Make a vector of pair, convert the unidirected graph into bidirected but the reverse direction should be given 1 as weight and original direction should be given 0, Now use a priority queue to traverse the array, just like a normal queue. Using dikjstra algo, find the shortest distance between the src and destination and return that. If it is equal to INT_MAX, which is the initilial value, return -1.</t>
   </si>
 </sst>
 </file>
@@ -2021,7 +2024,7 @@
   <dimension ref="A1:AF481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A382" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B410" sqref="B410"/>
+      <selection activeCell="L397" sqref="L397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6247,9 +6250,11 @@
         <v>380</v>
       </c>
       <c r="C393" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D393" s="12"/>
+        <v>465</v>
+      </c>
+      <c r="D393" s="12" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="394" spans="1:32" ht="21">
       <c r="A394" s="8" t="s">

</xml_diff>

<commit_message>
added coin problem with explaination inside the xl
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06CBEB1-52E2-4553-9FE8-4744BEB0514C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5A5071-74CA-4838-A7F0-31E5B6B41CDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="504">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1563,6 +1563,9 @@
   </si>
   <si>
     <t xml:space="preserve">Memoization: Make a choice digram for recursion, this will consist of if you can include the element in the knapsack or not, check if the weight of current item is less than or equal to toal weight, if it is, return the max of recursive call of the same function including the element (reduce the max Weight and n) or don;t include the element, this will oonly reduce n. And if the element's weight is more than current. don't include and call the function again with onoly n-1. for the DP part, initialize a global matrix and memset it to -1 in the main code. whenever you are going in any condition, make the matrix on basis of the dimension of the varibale inputs of the recurisie function. Here it will be W and n, make a matrix of W+1 and n+1 dimension and for every recurvie return, instead, store that value insdie that matrix,  before going into any call, check if the value foor that W and n is soomething else than the initalize mem set value of the matrix, if so directly return that   </t>
+  </si>
+  <si>
+    <t>Unbounded Knapsack: Make the choice diagram for the recursion, this will be two cases, one if the current elementt is less then remaining amount from total to be made, if it is less than or equal to the remaining amount (n), you can either decide to keep it in the knapsack or not, so you will have to calls, one you will decrement index(m) and other you will subtract current amount with the value at index m, aka S[m-1]. Base case will be if the amount (n) ==0, increment count by 1 hence return 1. else if the amoount if less than 0 or index m is less than equal to 0, don't increment count, return 0. For DP, make a table for size 10001 by 10001, initialize by -1, and whenever returning, just stoore the value at respective m and n ( to understand how to decide dimensions of dp see the below solution). if at any call the matrix(t) has any other value than -1 at m,n return that value without extending the recursion call.</t>
   </si>
 </sst>
 </file>
@@ -2026,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:AF481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D412" sqref="D412"/>
+    <sheetView tabSelected="1" topLeftCell="A400" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E423" sqref="E423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6420,7 +6423,10 @@
         <v>394</v>
       </c>
       <c r="C410" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="D410" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="411" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added subset sum function
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5A5071-74CA-4838-A7F0-31E5B6B41CDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7206AD-FA87-449C-8EC1-034A670FAAD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="0" yWindow="1560" windowWidth="23040" windowHeight="9108" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="506">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1566,6 +1566,12 @@
   </si>
   <si>
     <t>Unbounded Knapsack: Make the choice diagram for the recursion, this will be two cases, one if the current elementt is less then remaining amount from total to be made, if it is less than or equal to the remaining amount (n), you can either decide to keep it in the knapsack or not, so you will have to calls, one you will decrement index(m) and other you will subtract current amount with the value at index m, aka S[m-1]. Base case will be if the amount (n) ==0, increment count by 1 hence return 1. else if the amoount if less than 0 or index m is less than equal to 0, don't increment count, return 0. For DP, make a table for size 10001 by 10001, initialize by -1, and whenever returning, just stoore the value at respective m and n ( to understand how to decide dimensions of dp see the below solution). if at any call the matrix(t) has any other value than -1 at m,n return that value without extending the recursion call.</t>
+  </si>
+  <si>
+    <t>TopDown: Convert all the recursive function to a iterative function with the following steps. Convert the base condition in itilialization step. And convert the variable inputs into I and j as per the order of dimension. Please refer the the book notes for easier understanding</t>
+  </si>
+  <si>
+    <t>Bounded Knapsack: Similar to target sum justt change being that the target sum will be half, and the total sum of the array must be even. This is because if the sum is odd, you cannot divide it into two half of equal sum. And if you can find that one half exists with sum to equal to half of the total sum. Other must be equal to the rremainig from the total sum which is half sum again,</t>
   </si>
 </sst>
 </file>
@@ -2029,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:AF481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A400" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E423" sqref="E423"/>
+    <sheetView tabSelected="1" topLeftCell="A409" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B412" sqref="B412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6337,11 +6343,11 @@
       <c r="B400" s="7"/>
       <c r="C400" s="4"/>
     </row>
-    <row r="401" spans="1:4" ht="21">
+    <row r="401" spans="1:5" ht="21">
       <c r="B401" s="7"/>
       <c r="C401" s="4"/>
     </row>
-    <row r="402" spans="1:4" ht="21">
+    <row r="402" spans="1:5" ht="21">
       <c r="A402" s="8" t="s">
         <v>387</v>
       </c>
@@ -6352,7 +6358,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:4" ht="21">
+    <row r="403" spans="1:5" ht="21">
       <c r="A403" s="8" t="s">
         <v>387</v>
       </c>
@@ -6363,7 +6369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:4" ht="21">
+    <row r="404" spans="1:5" ht="21">
       <c r="A404" s="8" t="s">
         <v>387</v>
       </c>
@@ -6374,7 +6380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:4" ht="21">
+    <row r="405" spans="1:5" ht="21">
       <c r="A405" s="8" t="s">
         <v>387</v>
       </c>
@@ -6385,7 +6391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="406" spans="1:4" ht="21">
+    <row r="406" spans="1:5" ht="21">
       <c r="A406" s="8" t="s">
         <v>387</v>
       </c>
@@ -6396,7 +6402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:4" ht="21">
+    <row r="407" spans="1:5" ht="21">
       <c r="A407" s="8" t="s">
         <v>387</v>
       </c>
@@ -6407,15 +6413,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:4" ht="21">
+    <row r="408" spans="1:5" ht="21">
       <c r="B408" s="7"/>
       <c r="C408" s="4"/>
     </row>
-    <row r="409" spans="1:4" ht="21">
+    <row r="409" spans="1:5" ht="21">
       <c r="B409" s="7"/>
       <c r="C409" s="4"/>
     </row>
-    <row r="410" spans="1:4" ht="21">
+    <row r="410" spans="1:5" ht="21">
       <c r="A410" s="5" t="s">
         <v>393</v>
       </c>
@@ -6429,7 +6435,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="411" spans="1:4" ht="21">
+    <row r="411" spans="1:5" ht="21">
       <c r="A411" s="5" t="s">
         <v>393</v>
       </c>
@@ -6439,11 +6445,14 @@
       <c r="C411" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="D411" t="s">
+      <c r="D411" s="12" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="412" spans="1:4" ht="21">
+      <c r="E411" s="12" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" ht="21">
       <c r="A412" s="5" t="s">
         <v>393</v>
       </c>
@@ -6454,7 +6463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:4" ht="21">
+    <row r="413" spans="1:5" ht="21">
       <c r="A413" s="5" t="s">
         <v>393</v>
       </c>
@@ -6465,7 +6474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:4" ht="21">
+    <row r="414" spans="1:5" ht="21">
       <c r="A414" s="5" t="s">
         <v>393</v>
       </c>
@@ -6476,7 +6485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="415" spans="1:4" ht="21">
+    <row r="415" spans="1:5" ht="21">
       <c r="A415" s="5" t="s">
         <v>393</v>
       </c>
@@ -6487,7 +6496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="416" spans="1:4" ht="21">
+    <row r="416" spans="1:5" ht="21">
       <c r="A416" s="5" t="s">
         <v>393</v>
       </c>
@@ -6498,7 +6507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="21">
+    <row r="417" spans="1:4" ht="21">
       <c r="A417" s="5" t="s">
         <v>393</v>
       </c>
@@ -6506,10 +6515,13 @@
         <v>273</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="418" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D417" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" ht="21">
       <c r="A418" s="5" t="s">
         <v>393</v>
       </c>
@@ -6520,7 +6532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="21">
+    <row r="419" spans="1:4" ht="21">
       <c r="A419" s="5" t="s">
         <v>393</v>
       </c>
@@ -6531,7 +6543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420" spans="1:3" ht="21">
+    <row r="420" spans="1:4" ht="21">
       <c r="A420" s="5" t="s">
         <v>393</v>
       </c>
@@ -6542,7 +6554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="421" spans="1:3" ht="21">
+    <row r="421" spans="1:4" ht="21">
       <c r="A421" s="5" t="s">
         <v>393</v>
       </c>
@@ -6553,7 +6565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:3" ht="21">
+    <row r="422" spans="1:4" ht="21">
       <c r="A422" s="5" t="s">
         <v>393</v>
       </c>
@@ -6564,7 +6576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:3" ht="21">
+    <row r="423" spans="1:4" ht="21">
       <c r="A423" s="5" t="s">
         <v>393</v>
       </c>
@@ -6575,7 +6587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="424" spans="1:3" ht="21">
+    <row r="424" spans="1:4" ht="21">
       <c r="A424" s="5" t="s">
         <v>393</v>
       </c>
@@ -6586,7 +6598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="425" spans="1:3" ht="21">
+    <row r="425" spans="1:4" ht="21">
       <c r="A425" s="5" t="s">
         <v>393</v>
       </c>
@@ -6597,7 +6609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="426" spans="1:3" ht="21">
+    <row r="426" spans="1:4" ht="21">
       <c r="A426" s="5" t="s">
         <v>393</v>
       </c>
@@ -6608,7 +6620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:3" ht="21">
+    <row r="427" spans="1:4" ht="21">
       <c r="A427" s="5" t="s">
         <v>393</v>
       </c>
@@ -6619,7 +6631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="428" spans="1:3" ht="21">
+    <row r="428" spans="1:4" ht="21">
       <c r="A428" s="5" t="s">
         <v>393</v>
       </c>
@@ -6630,7 +6642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="21">
+    <row r="429" spans="1:4" ht="21">
       <c r="A429" s="5" t="s">
         <v>393</v>
       </c>
@@ -6641,7 +6653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="430" spans="1:3" ht="21">
+    <row r="430" spans="1:4" ht="21">
       <c r="A430" s="5" t="s">
         <v>393</v>
       </c>
@@ -6652,7 +6664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="431" spans="1:3" ht="21">
+    <row r="431" spans="1:4" ht="21">
       <c r="A431" s="5" t="s">
         <v>393</v>
       </c>
@@ -6663,7 +6675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="432" spans="1:3" ht="21">
+    <row r="432" spans="1:4" ht="21">
       <c r="A432" s="5" t="s">
         <v>393</v>
       </c>

</xml_diff>

<commit_message>
added top down for coin change
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07075C02-AC17-4FE0-B9E7-4D135361C107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D356C93-9E89-4B9A-8697-A99D54FF132C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2048,7 +2048,7 @@
   <dimension ref="A1:AF481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A397" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N407" sqref="N407"/>
+      <selection activeCell="K406" sqref="K406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
added bottom up solution for LCS
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D356C93-9E89-4B9A-8697-A99D54FF132C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3AB5F7-10FF-4E97-B3B5-E94106AE5BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="17775" yWindow="1965" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="511">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1584,6 +1584,9 @@
   </si>
   <si>
     <t>make a 1D array, initialize the first two spots with 1. loop from 2, and for each I in the loop, find summation of each pair element from 0 to I, where element one is at j and element 2 is at i-j-1, return the last space for output.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear Dp. Simple reucursion with the following formula  function(n-1)+(n-1)*function(n-2) .make a dp table for n+1 and assign them -1, if the value at n is not equal to -1 in recursive function return t[n] </t>
   </si>
 </sst>
 </file>
@@ -2048,17 +2051,17 @@
   <dimension ref="A1:AF481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A397" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K406" sqref="K406"/>
+      <selection activeCell="B421" sqref="B421"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6550,7 +6553,10 @@
         <v>401</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="D418" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="419" spans="1:4" ht="21">

</xml_diff>

<commit_message>
addeed code for lcs of three strings
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3AB5F7-10FF-4E97-B3B5-E94106AE5BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4F3464-86E9-49CF-8217-4B6DC813A1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17775" yWindow="1965" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="14220" yWindow="1560" windowWidth="8820" windowHeight="9108" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="513">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1587,6 +1587,12 @@
   </si>
   <si>
     <t xml:space="preserve">Linear Dp. Simple reucursion with the following formula  function(n-1)+(n-1)*function(n-2) .make a dp table for n+1 and assign them -1, if the value at n is not equal to -1 in recursive function return t[n] </t>
+  </si>
+  <si>
+    <t>LCS: Initialize matrix for i==0 || j==0 with 0. Loop through the matrix, if the elements at i-1 and jj-1 are same then increment count of the diagonally previous element, aka i-1,j-1. else take max of the vertically pervious or horizontal previous.aka (i-1,j) or (i,j-1) return the last element</t>
+  </si>
+  <si>
+    <t>Same as longest common subsequence, but as substrings have to be continuous , when ever the characters are not matching and the code goes in the else condition, instead of max of two elements, reset the count to 0. After wards traverse the entire matrix to find the max element and return that</t>
   </si>
 </sst>
 </file>
@@ -2050,8 +2056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:AF481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A397" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B421" sqref="B421"/>
+    <sheetView tabSelected="1" topLeftCell="B419" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B436" sqref="B436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -6614,7 +6620,10 @@
         <v>406</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="D423" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="21">
@@ -6716,7 +6725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="433" spans="1:3" ht="21">
+    <row r="433" spans="1:4" ht="21">
       <c r="A433" s="5" t="s">
         <v>393</v>
       </c>
@@ -6727,7 +6736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="434" spans="1:3" ht="21">
+    <row r="434" spans="1:4" ht="21">
       <c r="A434" s="5" t="s">
         <v>393</v>
       </c>
@@ -6738,7 +6747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:3" ht="21">
+    <row r="435" spans="1:4" ht="21">
       <c r="A435" s="5" t="s">
         <v>393</v>
       </c>
@@ -6749,7 +6758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:3" ht="21">
+    <row r="436" spans="1:4" ht="21">
       <c r="A436" s="5" t="s">
         <v>393</v>
       </c>
@@ -6760,7 +6769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="437" spans="1:3" ht="21">
+    <row r="437" spans="1:4" ht="21">
       <c r="A437" s="5" t="s">
         <v>393</v>
       </c>
@@ -6771,7 +6780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="438" spans="1:3" ht="21">
+    <row r="438" spans="1:4" ht="21">
       <c r="A438" s="5" t="s">
         <v>393</v>
       </c>
@@ -6782,7 +6791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="439" spans="1:3" ht="21">
+    <row r="439" spans="1:4" ht="21">
       <c r="A439" s="5" t="s">
         <v>393</v>
       </c>
@@ -6793,7 +6802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:3" ht="21">
+    <row r="440" spans="1:4" ht="21">
       <c r="A440" s="5" t="s">
         <v>393</v>
       </c>
@@ -6804,7 +6813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="441" spans="1:3" ht="21">
+    <row r="441" spans="1:4" ht="21">
       <c r="A441" s="5" t="s">
         <v>393</v>
       </c>
@@ -6812,10 +6821,13 @@
         <v>424</v>
       </c>
       <c r="C441" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="442" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D441" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" ht="21">
       <c r="A442" s="5" t="s">
         <v>393</v>
       </c>
@@ -6826,7 +6838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:3" ht="21">
+    <row r="443" spans="1:4" ht="21">
       <c r="A443" s="5" t="s">
         <v>393</v>
       </c>
@@ -6837,7 +6849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="444" spans="1:3" ht="21">
+    <row r="444" spans="1:4" ht="21">
       <c r="A444" s="5" t="s">
         <v>393</v>
       </c>
@@ -6848,7 +6860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="445" spans="1:3" ht="21">
+    <row r="445" spans="1:4" ht="21">
       <c r="A445" s="5" t="s">
         <v>393</v>
       </c>
@@ -6859,7 +6871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="446" spans="1:3" ht="21">
+    <row r="446" spans="1:4" ht="21">
       <c r="A446" s="5" t="s">
         <v>393</v>
       </c>
@@ -6870,7 +6882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="447" spans="1:3" ht="21">
+    <row r="447" spans="1:4" ht="21">
       <c r="A447" s="5" t="s">
         <v>393</v>
       </c>
@@ -6881,7 +6893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="448" spans="1:3" ht="21">
+    <row r="448" spans="1:4" ht="21">
       <c r="A448" s="5" t="s">
         <v>393</v>
       </c>

</xml_diff>

<commit_message>
added longest increasing code
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2617091B-D529-4411-91A5-7FB514E3330C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B64B07-E6BB-4215-8EC4-E74EEE4FC49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="517">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1596,6 +1596,15 @@
   </si>
   <si>
     <t>Same as LCS of two strings but now it will have three dimensions. M n p where p will be the length of the third string. If elements of all the strings at end are same , decrement m n and p by 1, else take max of the recursive call for m-1, n-1 and p-1 seperately.</t>
+  </si>
+  <si>
+    <t>Init the matrix with I and j on each row and col instead of 0, if the elements are same don't compy the digonally previous element, else take minimum from up, left and up-left element and add one. Return t[n][m]</t>
+  </si>
+  <si>
+    <t>Reverse the string and find the lcs between the new reversed string and the orignal string, this will be the length of longest palindromic subsequence</t>
+  </si>
+  <si>
+    <t>Make a new vector that is sorted and does not contain any duplicates from the first vector. Take lcs between these two vectors and you will find the sum, instead of adding 1 to the count, add the current interger being compared.</t>
   </si>
 </sst>
 </file>
@@ -2059,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:AF481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B425" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G431" sqref="G431"/>
+    <sheetView tabSelected="1" topLeftCell="A422" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H431" sqref="H431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6537,7 +6546,10 @@
         <v>400</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="D416" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="417" spans="1:4" ht="21">
@@ -6684,7 +6696,10 @@
         <v>411</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="D428" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="429" spans="1:4" ht="21">
@@ -6910,7 +6925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="449" spans="1:3" ht="21">
+    <row r="449" spans="1:4" ht="21">
       <c r="A449" s="5" t="s">
         <v>393</v>
       </c>
@@ -6921,7 +6936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="450" spans="1:3" ht="21">
+    <row r="450" spans="1:4" ht="21">
       <c r="A450" s="5" t="s">
         <v>393</v>
       </c>
@@ -6929,10 +6944,13 @@
         <v>433</v>
       </c>
       <c r="C450" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="451" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D450" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" ht="21">
       <c r="A451" s="5" t="s">
         <v>393</v>
       </c>
@@ -6943,7 +6961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="452" spans="1:3" ht="21">
+    <row r="452" spans="1:4" ht="21">
       <c r="A452" s="5" t="s">
         <v>393</v>
       </c>
@@ -6954,7 +6972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="453" spans="1:3" ht="21">
+    <row r="453" spans="1:4" ht="21">
       <c r="A453" s="5" t="s">
         <v>393</v>
       </c>
@@ -6965,7 +6983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="454" spans="1:3" ht="21">
+    <row r="454" spans="1:4" ht="21">
       <c r="A454" s="5" t="s">
         <v>393</v>
       </c>
@@ -6976,7 +6994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="455" spans="1:3" ht="21">
+    <row r="455" spans="1:4" ht="21">
       <c r="A455" s="5" t="s">
         <v>393</v>
       </c>
@@ -6987,7 +7005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="456" spans="1:3" ht="21">
+    <row r="456" spans="1:4" ht="21">
       <c r="A456" s="5" t="s">
         <v>393</v>
       </c>
@@ -6998,7 +7016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="457" spans="1:3" ht="21">
+    <row r="457" spans="1:4" ht="21">
       <c r="A457" s="5" t="s">
         <v>393</v>
       </c>
@@ -7009,7 +7027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="458" spans="1:3" ht="21">
+    <row r="458" spans="1:4" ht="21">
       <c r="A458" s="5" t="s">
         <v>393</v>
       </c>
@@ -7020,7 +7038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="459" spans="1:3" ht="21">
+    <row r="459" spans="1:4" ht="21">
       <c r="A459" s="5" t="s">
         <v>393</v>
       </c>
@@ -7031,7 +7049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="460" spans="1:3" ht="21">
+    <row r="460" spans="1:4" ht="21">
       <c r="A460" s="5" t="s">
         <v>393</v>
       </c>
@@ -7042,7 +7060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="461" spans="1:3" ht="21">
+    <row r="461" spans="1:4" ht="21">
       <c r="A461" s="5" t="s">
         <v>393</v>
       </c>
@@ -7053,7 +7071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="462" spans="1:3" ht="21">
+    <row r="462" spans="1:4" ht="21">
       <c r="A462" s="5" t="s">
         <v>393</v>
       </c>
@@ -7064,7 +7082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="463" spans="1:3" ht="21">
+    <row r="463" spans="1:4" ht="21">
       <c r="A463" s="5" t="s">
         <v>393</v>
       </c>
@@ -7075,7 +7093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="464" spans="1:3" ht="21">
+    <row r="464" spans="1:4" ht="21">
       <c r="A464" s="5" t="s">
         <v>393</v>
       </c>

</xml_diff>

<commit_message>
added ways to reach score solution
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D23AA2B-DFDA-44CF-B960-C008828FB5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE38D68C-73E1-423B-9A24-17B3716F9BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2812" uniqueCount="527">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1629,6 +1629,12 @@
   </si>
   <si>
     <t>Another optimization on this by using binary search instead of looping from j=1 to k.</t>
+  </si>
+  <si>
+    <t>Simple alteration of the kadane algorrithm, instead of resetting the sum to 0 when it goes below 0. we set the temp sum to the element at hand if the temp sum goes above 0. and take the minimum of each iteration</t>
+  </si>
+  <si>
+    <t>make a table for n+1, loop for each case of I as 3 5 10, for each valur of table[i], add the value of table[i-3],table[i-5] and table[i-10] respectively and return the last element</t>
   </si>
 </sst>
 </file>
@@ -2092,18 +2098,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR426" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BI438" sqref="BI438"/>
+    <sheetView tabSelected="1" topLeftCell="A422" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B449" sqref="B449"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6895,7 +6901,10 @@
         <v>425</v>
       </c>
       <c r="C442" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="D442" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="443" spans="1:4" ht="21">
@@ -6931,7 +6940,10 @@
         <v>428</v>
       </c>
       <c r="C445" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="D445" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="446" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added stack using queue with explaination
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC52B929-0423-499D-8C70-C239B63D47AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88561F90-D891-40B5-920F-270C73D50D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29760" yWindow="960" windowWidth="28800" windowHeight="11325" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="530">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1641,6 +1641,9 @@
   </si>
   <si>
     <t>The number of ways to paint one fence with k colours is k. The number of ways to paint two fence with k colours is k*k. This will be the base condition, anything above this will be (k-1)*(number of ways to paint n-1 fence + number of ways to paint n-2 fence). Memoization can be done with one directional array</t>
+  </si>
+  <si>
+    <t>Make two queues, whenever you need to push something, empty first queue and place all elements in queue two, then push the new int in queue 1, now empty queue 2 and place all elements in queue 1</t>
   </si>
 </sst>
 </file>
@@ -2104,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A404" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D422" sqref="D422"/>
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D313" sqref="D313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5308,7 +5311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:3" ht="21">
+    <row r="305" spans="1:4" ht="21">
       <c r="A305" s="5" t="s">
         <v>285</v>
       </c>
@@ -5319,7 +5322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:3" ht="21">
+    <row r="306" spans="1:4" ht="21">
       <c r="A306" s="5" t="s">
         <v>285</v>
       </c>
@@ -5330,7 +5333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="307" spans="1:3" ht="21">
+    <row r="307" spans="1:4" ht="21">
       <c r="A307" s="5" t="s">
         <v>285</v>
       </c>
@@ -5341,7 +5344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="308" spans="1:3" ht="21">
+    <row r="308" spans="1:4" ht="21">
       <c r="A308" s="5" t="s">
         <v>285</v>
       </c>
@@ -5352,7 +5355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="309" spans="1:3" ht="21">
+    <row r="309" spans="1:4" ht="21">
       <c r="A309" s="5" t="s">
         <v>285</v>
       </c>
@@ -5363,7 +5366,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="310" spans="1:3" ht="21">
+    <row r="310" spans="1:4" ht="21">
       <c r="A310" s="5" t="s">
         <v>285</v>
       </c>
@@ -5374,7 +5377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="311" spans="1:3" ht="21">
+    <row r="311" spans="1:4" ht="21">
       <c r="A311" s="5" t="s">
         <v>285</v>
       </c>
@@ -5385,7 +5388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="312" spans="1:3" ht="21">
+    <row r="312" spans="1:4" ht="21">
       <c r="A312" s="5" t="s">
         <v>285</v>
       </c>
@@ -5396,7 +5399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="313" spans="1:3" ht="21">
+    <row r="313" spans="1:4" ht="21">
       <c r="A313" s="5" t="s">
         <v>285</v>
       </c>
@@ -5407,7 +5410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="314" spans="1:3" ht="21">
+    <row r="314" spans="1:4" ht="21">
       <c r="A314" s="5" t="s">
         <v>285</v>
       </c>
@@ -5418,7 +5421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="315" spans="1:3" ht="21">
+    <row r="315" spans="1:4" ht="21">
       <c r="A315" s="5" t="s">
         <v>285</v>
       </c>
@@ -5426,10 +5429,13 @@
         <v>305</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D315" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" ht="21">
       <c r="A316" s="5" t="s">
         <v>285</v>
       </c>
@@ -5440,7 +5446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="317" spans="1:3" ht="21">
+    <row r="317" spans="1:4" ht="21">
       <c r="A317" s="5" t="s">
         <v>285</v>
       </c>
@@ -5451,7 +5457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="318" spans="1:3" ht="21">
+    <row r="318" spans="1:4" ht="21">
       <c r="A318" s="5" t="s">
         <v>285</v>
       </c>
@@ -5462,7 +5468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="319" spans="1:3" ht="21">
+    <row r="319" spans="1:4" ht="21">
       <c r="A319" s="5" t="s">
         <v>285</v>
       </c>
@@ -5473,7 +5479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="320" spans="1:3" ht="21">
+    <row r="320" spans="1:4" ht="21">
       <c r="A320" s="5" t="s">
         <v>285</v>
       </c>

</xml_diff>

<commit_message>
adding explanation of arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32ECA81-B770-4C9B-B375-DAB50A07811B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD523DD-75D1-4A4F-80F3-EDA72B146297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="28800" windowHeight="11325" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11325" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1434,16 +1434,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>9 mins</t>
-  </si>
-  <si>
     <t xml:space="preserve">time </t>
-  </si>
-  <si>
-    <t>1 min</t>
-  </si>
-  <si>
-    <t>3 mins</t>
   </si>
   <si>
     <t>no</t>
@@ -1647,6 +1638,15 @@
   </si>
   <si>
     <t>Make two queues, whenever you need to push something, empty first queue and place all elements in queue two, then push the new int in queue 1, now empty queue 2 and place all elements in queue 1, for pop, simpy return the top element of the queue using front</t>
+  </si>
+  <si>
+    <t>Simple print from i=n-1 to 0 if you just wanna print, if you wanna reverse use a stack or you can reverse from the middle using two pointer.</t>
+  </si>
+  <si>
+    <t>sort the array and return the value at k-1 for smallest and n-k-1 for the largest</t>
+  </si>
+  <si>
+    <t>Initialize the minimum and maximum value with INT_MAX and INT_MIN respectively and loop the array to find min of element and minimum value and same with max, if aany value is less than minimum replace it with min, same with max</t>
   </si>
 </sst>
 </file>
@@ -2110,18 +2110,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D316" sqref="D316"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2161,7 +2161,7 @@
         <v>465</v>
       </c>
       <c r="D6" t="s">
-        <v>466</v>
+        <v>528</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21">
@@ -2175,7 +2175,7 @@
         <v>465</v>
       </c>
       <c r="D7" t="s">
-        <v>468</v>
+        <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21">
@@ -2189,7 +2189,7 @@
         <v>465</v>
       </c>
       <c r="D8" t="s">
-        <v>469</v>
+        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21">
@@ -2258,7 +2258,7 @@
         <v>465</v>
       </c>
       <c r="D14" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2619,7 +2619,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="21">
@@ -2630,7 +2630,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21">
@@ -2641,7 +2641,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">
@@ -2663,7 +2663,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="21">
@@ -2674,7 +2674,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="21">
@@ -2778,7 +2778,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">
@@ -2822,7 +2822,7 @@
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="21">
@@ -2833,7 +2833,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="21">
@@ -2866,7 +2866,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="21">
@@ -2954,7 +2954,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="21">
@@ -3223,7 +3223,7 @@
         <v>103</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="21">
@@ -3278,7 +3278,7 @@
         <v>108</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="21">
@@ -3377,7 +3377,7 @@
         <v>117</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="21">
@@ -3454,7 +3454,7 @@
         <v>124</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="21">
@@ -4976,7 +4976,7 @@
         <v>87</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="21">
@@ -5435,7 +5435,7 @@
         <v>465</v>
       </c>
       <c r="D315" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="21">
@@ -5471,7 +5471,7 @@
         <v>465</v>
       </c>
       <c r="D318" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="21">
@@ -5952,7 +5952,7 @@
         <v>465</v>
       </c>
       <c r="D364" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="21">
@@ -5966,7 +5966,7 @@
         <v>465</v>
       </c>
       <c r="D365" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="21">
@@ -5980,7 +5980,7 @@
         <v>465</v>
       </c>
       <c r="D366" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="367" spans="1:4" ht="21">
@@ -5994,7 +5994,7 @@
         <v>465</v>
       </c>
       <c r="D367" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="21">
@@ -6008,7 +6008,7 @@
         <v>465</v>
       </c>
       <c r="D368" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="369" spans="1:29" ht="21">
@@ -6022,7 +6022,7 @@
         <v>465</v>
       </c>
       <c r="D369" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="370" spans="1:29" ht="21">
@@ -6036,7 +6036,7 @@
         <v>465</v>
       </c>
       <c r="D370" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="371" spans="1:29" ht="21">
@@ -6050,7 +6050,7 @@
         <v>465</v>
       </c>
       <c r="D371" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="372" spans="1:29" ht="21">
@@ -6086,7 +6086,7 @@
         <v>465</v>
       </c>
       <c r="D374" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="375" spans="1:29" ht="21">
@@ -6100,7 +6100,7 @@
         <v>465</v>
       </c>
       <c r="D375" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="376" spans="1:29" ht="21">
@@ -6114,7 +6114,7 @@
         <v>465</v>
       </c>
       <c r="D376" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="377" spans="1:29" ht="21">
@@ -6128,7 +6128,7 @@
         <v>465</v>
       </c>
       <c r="D377" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="378" spans="1:29" ht="21">
@@ -6139,7 +6139,7 @@
         <v>366</v>
       </c>
       <c r="C378" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="379" spans="1:29" ht="21">
@@ -6164,10 +6164,10 @@
         <v>465</v>
       </c>
       <c r="D380" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="AC380" s="12" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="381" spans="1:29" ht="21">
@@ -6181,7 +6181,7 @@
         <v>465</v>
       </c>
       <c r="D381" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="382" spans="1:29" ht="21">
@@ -6206,7 +6206,7 @@
         <v>465</v>
       </c>
       <c r="D383" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="384" spans="1:29" ht="21">
@@ -6220,7 +6220,7 @@
         <v>465</v>
       </c>
       <c r="D384" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="385" spans="1:32" ht="21">
@@ -6234,7 +6234,7 @@
         <v>465</v>
       </c>
       <c r="D385" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="386" spans="1:32" ht="21">
@@ -6248,10 +6248,10 @@
         <v>465</v>
       </c>
       <c r="D386" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="AF386" s="12" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="387" spans="1:32" ht="21">
@@ -6265,7 +6265,7 @@
         <v>465</v>
       </c>
       <c r="D387" s="12" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="388" spans="1:32" ht="21">
@@ -6279,7 +6279,7 @@
         <v>465</v>
       </c>
       <c r="D388" s="12" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="389" spans="1:32" ht="21">
@@ -6293,7 +6293,7 @@
         <v>465</v>
       </c>
       <c r="D389" s="12" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="390" spans="1:32" ht="21">
@@ -6307,7 +6307,7 @@
         <v>465</v>
       </c>
       <c r="D390" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="391" spans="1:32" ht="21">
@@ -6321,7 +6321,7 @@
         <v>465</v>
       </c>
       <c r="D391" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="392" spans="1:32" ht="21">
@@ -6335,7 +6335,7 @@
         <v>465</v>
       </c>
       <c r="D392" s="12" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="393" spans="1:32" ht="21">
@@ -6349,7 +6349,7 @@
         <v>465</v>
       </c>
       <c r="D393" s="12" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="394" spans="1:32" ht="21">
@@ -6360,7 +6360,7 @@
         <v>381</v>
       </c>
       <c r="C394" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D394" s="12"/>
     </row>
@@ -6516,7 +6516,7 @@
         <v>465</v>
       </c>
       <c r="D410" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="411" spans="1:5" ht="21">
@@ -6530,10 +6530,10 @@
         <v>465</v>
       </c>
       <c r="D411" s="12" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E411" s="12" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="412" spans="1:5" ht="21">
@@ -6547,7 +6547,7 @@
         <v>465</v>
       </c>
       <c r="D412" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="413" spans="1:5" ht="21">
@@ -6561,7 +6561,7 @@
         <v>465</v>
       </c>
       <c r="D413" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="414" spans="1:5" ht="21">
@@ -6575,7 +6575,7 @@
         <v>465</v>
       </c>
       <c r="D414" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="415" spans="1:5" ht="21">
@@ -6589,7 +6589,7 @@
         <v>465</v>
       </c>
       <c r="D415" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="416" spans="1:5" ht="21">
@@ -6603,7 +6603,7 @@
         <v>465</v>
       </c>
       <c r="D416" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="417" spans="1:66" ht="21">
@@ -6617,7 +6617,7 @@
         <v>465</v>
       </c>
       <c r="D417" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="418" spans="1:66" ht="21">
@@ -6631,7 +6631,7 @@
         <v>465</v>
       </c>
       <c r="D418" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="419" spans="1:66" ht="21">
@@ -6645,7 +6645,7 @@
         <v>465</v>
       </c>
       <c r="D419" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="420" spans="1:66" ht="21">
@@ -6670,7 +6670,7 @@
         <v>465</v>
       </c>
       <c r="D421" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="422" spans="1:66" ht="21">
@@ -6684,7 +6684,7 @@
         <v>465</v>
       </c>
       <c r="D422" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="423" spans="1:66" ht="21">
@@ -6698,7 +6698,7 @@
         <v>465</v>
       </c>
       <c r="D423" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="424" spans="1:66" ht="21">
@@ -6712,7 +6712,7 @@
         <v>465</v>
       </c>
       <c r="D424" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="425" spans="1:66" ht="21">
@@ -6748,7 +6748,7 @@
         <v>465</v>
       </c>
       <c r="D427" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="428" spans="1:66" ht="21">
@@ -6762,7 +6762,7 @@
         <v>465</v>
       </c>
       <c r="D428" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="429" spans="1:66" ht="21">
@@ -6809,10 +6809,10 @@
         <v>465</v>
       </c>
       <c r="D432" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="BN432" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="433" spans="1:4" ht="21">
@@ -6914,7 +6914,7 @@
         <v>465</v>
       </c>
       <c r="D441" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="442" spans="1:4" ht="21">
@@ -6928,7 +6928,7 @@
         <v>465</v>
       </c>
       <c r="D442" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="443" spans="1:4" ht="21">
@@ -6953,7 +6953,7 @@
         <v>465</v>
       </c>
       <c r="D444" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="445" spans="1:4" ht="21">
@@ -6967,7 +6967,7 @@
         <v>465</v>
       </c>
       <c r="D445" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="446" spans="1:4" ht="21">
@@ -7025,7 +7025,7 @@
         <v>465</v>
       </c>
       <c r="D450" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="451" spans="1:4" ht="21">
@@ -7138,7 +7138,7 @@
         <v>465</v>
       </c>
       <c r="D460" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="461" spans="1:4" ht="21">
@@ -7174,7 +7174,7 @@
         <v>465</v>
       </c>
       <c r="D463" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="464" spans="1:4" ht="21">

</xml_diff>

<commit_message>
0,1,2 sorting explanation addedd
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD523DD-75D1-4A4F-80F3-EDA72B146297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED366BB-5D2A-4296-B151-C09BD907A4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11325" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="532">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1647,6 +1647,9 @@
   </si>
   <si>
     <t>Initialize the minimum and maximum value with INT_MAX and INT_MIN respectively and loop the array to find min of element and minimum value and same with max, if aany value is less than minimum replace it with min, same with max</t>
+  </si>
+  <si>
+    <t>Make a counter for 1,2 and 0. Traverse the array and count the number. Once done, make three while loops and decrement 0 , 1  and 2 in that order, placec each of these element inside the location of I in the array increment I on each placement</t>
   </si>
 </sst>
 </file>
@@ -2111,7 +2114,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2201,6 +2204,9 @@
       </c>
       <c r="C9" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D9" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">

</xml_diff>

<commit_message>
revision of array: move negative
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED366BB-5D2A-4296-B151-C09BD907A4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E16C78-E3FD-446F-AC44-2F1216A9286E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11325" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="533">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1650,6 +1650,9 @@
   </si>
   <si>
     <t>Make a counter for 1,2 and 0. Traverse the array and count the number. Once done, make three while loops and decrement 0 , 1  and 2 in that order, placec each of these element inside the location of I in the array increment I on each placement</t>
+  </si>
+  <si>
+    <t>Make two stacks to hold the elements, traverse the array and store positive in one and negative in other. Once done, reverse traverse the arrray and empty the negative stack first, oncee that is empty, start emptying the pos stack</t>
   </si>
 </sst>
 </file>
@@ -2114,7 +2117,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2218,6 +2221,9 @@
       </c>
       <c r="C10" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D10" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">

</xml_diff>

<commit_message>
array rivision: union find
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E16C78-E3FD-446F-AC44-2F1216A9286E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BE54C9-0221-43B3-90AE-8763DE78CAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11325" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="534">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1432,9 +1432,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time </t>
   </si>
   <si>
     <t>no</t>
@@ -1653,6 +1650,12 @@
   </si>
   <si>
     <t>Make two stacks to hold the elements, traverse the array and store positive in one and negative in other. Once done, reverse traverse the arrray and empty the negative stack first, oncee that is empty, start emptying the pos stack</t>
+  </si>
+  <si>
+    <t>Explaination</t>
+  </si>
+  <si>
+    <t>Make an unordered_set and traverse both the arrys and return the size of the set in the end of the function</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2120,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2148,7 +2151,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>466</v>
+        <v>532</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2167,7 +2170,7 @@
         <v>465</v>
       </c>
       <c r="D6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21">
@@ -2181,7 +2184,7 @@
         <v>465</v>
       </c>
       <c r="D7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21">
@@ -2195,7 +2198,7 @@
         <v>465</v>
       </c>
       <c r="D8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21">
@@ -2209,7 +2212,7 @@
         <v>465</v>
       </c>
       <c r="D9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">
@@ -2223,7 +2226,7 @@
         <v>465</v>
       </c>
       <c r="D10" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
@@ -2236,6 +2239,9 @@
       <c r="C11" s="4" t="s">
         <v>465</v>
       </c>
+      <c r="D11" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="21">
       <c r="A12" s="5" t="s">
@@ -2270,7 +2276,7 @@
         <v>465</v>
       </c>
       <c r="D14" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2631,7 +2637,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="21">
@@ -2642,7 +2648,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21">
@@ -2653,7 +2659,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">
@@ -2675,7 +2681,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="21">
@@ -2686,7 +2692,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="21">
@@ -2790,7 +2796,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">
@@ -2834,7 +2840,7 @@
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="21">
@@ -2845,7 +2851,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="21">
@@ -2878,7 +2884,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="21">
@@ -2966,7 +2972,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="21">
@@ -3235,7 +3241,7 @@
         <v>103</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="21">
@@ -3290,7 +3296,7 @@
         <v>108</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="21">
@@ -3389,7 +3395,7 @@
         <v>117</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="21">
@@ -3466,7 +3472,7 @@
         <v>124</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="21">
@@ -4988,7 +4994,7 @@
         <v>87</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="21">
@@ -5447,7 +5453,7 @@
         <v>465</v>
       </c>
       <c r="D315" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="21">
@@ -5483,7 +5489,7 @@
         <v>465</v>
       </c>
       <c r="D318" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="21">
@@ -5964,7 +5970,7 @@
         <v>465</v>
       </c>
       <c r="D364" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="21">
@@ -5978,7 +5984,7 @@
         <v>465</v>
       </c>
       <c r="D365" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="21">
@@ -5992,7 +5998,7 @@
         <v>465</v>
       </c>
       <c r="D366" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="367" spans="1:4" ht="21">
@@ -6006,7 +6012,7 @@
         <v>465</v>
       </c>
       <c r="D367" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="21">
@@ -6020,7 +6026,7 @@
         <v>465</v>
       </c>
       <c r="D368" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="369" spans="1:29" ht="21">
@@ -6034,7 +6040,7 @@
         <v>465</v>
       </c>
       <c r="D369" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="370" spans="1:29" ht="21">
@@ -6048,7 +6054,7 @@
         <v>465</v>
       </c>
       <c r="D370" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="371" spans="1:29" ht="21">
@@ -6062,7 +6068,7 @@
         <v>465</v>
       </c>
       <c r="D371" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="372" spans="1:29" ht="21">
@@ -6098,7 +6104,7 @@
         <v>465</v>
       </c>
       <c r="D374" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="375" spans="1:29" ht="21">
@@ -6112,7 +6118,7 @@
         <v>465</v>
       </c>
       <c r="D375" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="376" spans="1:29" ht="21">
@@ -6126,7 +6132,7 @@
         <v>465</v>
       </c>
       <c r="D376" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="377" spans="1:29" ht="21">
@@ -6140,7 +6146,7 @@
         <v>465</v>
       </c>
       <c r="D377" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="378" spans="1:29" ht="21">
@@ -6151,7 +6157,7 @@
         <v>366</v>
       </c>
       <c r="C378" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="379" spans="1:29" ht="21">
@@ -6176,10 +6182,10 @@
         <v>465</v>
       </c>
       <c r="D380" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AC380" s="12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="381" spans="1:29" ht="21">
@@ -6193,7 +6199,7 @@
         <v>465</v>
       </c>
       <c r="D381" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="382" spans="1:29" ht="21">
@@ -6218,7 +6224,7 @@
         <v>465</v>
       </c>
       <c r="D383" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="384" spans="1:29" ht="21">
@@ -6232,7 +6238,7 @@
         <v>465</v>
       </c>
       <c r="D384" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="385" spans="1:32" ht="21">
@@ -6246,7 +6252,7 @@
         <v>465</v>
       </c>
       <c r="D385" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="386" spans="1:32" ht="21">
@@ -6260,10 +6266,10 @@
         <v>465</v>
       </c>
       <c r="D386" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AF386" s="12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="387" spans="1:32" ht="21">
@@ -6277,7 +6283,7 @@
         <v>465</v>
       </c>
       <c r="D387" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="388" spans="1:32" ht="21">
@@ -6291,7 +6297,7 @@
         <v>465</v>
       </c>
       <c r="D388" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="389" spans="1:32" ht="21">
@@ -6305,7 +6311,7 @@
         <v>465</v>
       </c>
       <c r="D389" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="390" spans="1:32" ht="21">
@@ -6319,7 +6325,7 @@
         <v>465</v>
       </c>
       <c r="D390" s="12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="391" spans="1:32" ht="21">
@@ -6333,7 +6339,7 @@
         <v>465</v>
       </c>
       <c r="D391" s="12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="392" spans="1:32" ht="21">
@@ -6347,7 +6353,7 @@
         <v>465</v>
       </c>
       <c r="D392" s="12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="393" spans="1:32" ht="21">
@@ -6361,7 +6367,7 @@
         <v>465</v>
       </c>
       <c r="D393" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="394" spans="1:32" ht="21">
@@ -6372,7 +6378,7 @@
         <v>381</v>
       </c>
       <c r="C394" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D394" s="12"/>
     </row>
@@ -6528,7 +6534,7 @@
         <v>465</v>
       </c>
       <c r="D410" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="411" spans="1:5" ht="21">
@@ -6542,10 +6548,10 @@
         <v>465</v>
       </c>
       <c r="D411" s="12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E411" s="12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="412" spans="1:5" ht="21">
@@ -6559,7 +6565,7 @@
         <v>465</v>
       </c>
       <c r="D412" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="413" spans="1:5" ht="21">
@@ -6573,7 +6579,7 @@
         <v>465</v>
       </c>
       <c r="D413" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="414" spans="1:5" ht="21">
@@ -6587,7 +6593,7 @@
         <v>465</v>
       </c>
       <c r="D414" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="415" spans="1:5" ht="21">
@@ -6601,7 +6607,7 @@
         <v>465</v>
       </c>
       <c r="D415" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="416" spans="1:5" ht="21">
@@ -6615,7 +6621,7 @@
         <v>465</v>
       </c>
       <c r="D416" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="417" spans="1:66" ht="21">
@@ -6629,7 +6635,7 @@
         <v>465</v>
       </c>
       <c r="D417" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="418" spans="1:66" ht="21">
@@ -6643,7 +6649,7 @@
         <v>465</v>
       </c>
       <c r="D418" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="419" spans="1:66" ht="21">
@@ -6657,7 +6663,7 @@
         <v>465</v>
       </c>
       <c r="D419" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="420" spans="1:66" ht="21">
@@ -6682,7 +6688,7 @@
         <v>465</v>
       </c>
       <c r="D421" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="422" spans="1:66" ht="21">
@@ -6696,7 +6702,7 @@
         <v>465</v>
       </c>
       <c r="D422" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="423" spans="1:66" ht="21">
@@ -6710,7 +6716,7 @@
         <v>465</v>
       </c>
       <c r="D423" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="424" spans="1:66" ht="21">
@@ -6724,7 +6730,7 @@
         <v>465</v>
       </c>
       <c r="D424" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="425" spans="1:66" ht="21">
@@ -6760,7 +6766,7 @@
         <v>465</v>
       </c>
       <c r="D427" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="428" spans="1:66" ht="21">
@@ -6774,7 +6780,7 @@
         <v>465</v>
       </c>
       <c r="D428" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="429" spans="1:66" ht="21">
@@ -6821,10 +6827,10 @@
         <v>465</v>
       </c>
       <c r="D432" t="s">
+        <v>519</v>
+      </c>
+      <c r="BN432" t="s">
         <v>520</v>
-      </c>
-      <c r="BN432" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="433" spans="1:4" ht="21">
@@ -6926,7 +6932,7 @@
         <v>465</v>
       </c>
       <c r="D441" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="442" spans="1:4" ht="21">
@@ -6940,7 +6946,7 @@
         <v>465</v>
       </c>
       <c r="D442" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="443" spans="1:4" ht="21">
@@ -6965,7 +6971,7 @@
         <v>465</v>
       </c>
       <c r="D444" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="445" spans="1:4" ht="21">
@@ -6979,7 +6985,7 @@
         <v>465</v>
       </c>
       <c r="D445" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="446" spans="1:4" ht="21">
@@ -7037,7 +7043,7 @@
         <v>465</v>
       </c>
       <c r="D450" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="451" spans="1:4" ht="21">
@@ -7150,7 +7156,7 @@
         <v>465</v>
       </c>
       <c r="D460" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="461" spans="1:4" ht="21">
@@ -7186,7 +7192,7 @@
         <v>465</v>
       </c>
       <c r="D463" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="464" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added solution and explaintion of edit distance
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8FC178-63FE-4B50-973A-65C6347FC3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F48931-C90D-4388-AD04-394CF04F419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9024" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="537">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1438,9 +1438,6 @@
   </si>
   <si>
     <t>done with greedy/no</t>
-  </si>
-  <si>
-    <t>non optimised/no</t>
   </si>
   <si>
     <t>dp</t>
@@ -1665,6 +1662,9 @@
   </si>
   <si>
     <t>Used dp, initalize a matrix  with size of n+1,m+1 where n and m are the length of the wild string and pattern string respectively.  Set all elements to 0 using memset. Set first element to 1 as they match , aka both are empty string: "" "". Loop the dimension of wild and for all values of * place true as it matches to "" as per question. Now loop through the array from 1 to n+1 and from 1 to m+1, if the elements at wild[i-1]==pattern[j-1], set t[i][j] = t[i-1][j-1]. this is also true if wild[i-1] is '?' , if wild[i-1] is equal to *,  take the or of i-1,j and i,j-1. return the value at t[n][m] for ans</t>
+  </si>
+  <si>
+    <t>Done with DP: int the matrix with n+1 and m+1 where n and m are the length of s and t respectively. Now init the value at t[0][0] as 0 because both strings are equal. Now from i=0 to n+1, place t[i][0] = I and for j=0 to m+1 place t[0][j]=j. Now traverslse the matrix from 1 to n+1 and for j= 1 to m+1. For any point where s[i-1]==t[j-1], take the diagonally previous element at t[i-1][j-1] and place in t[i][j] else take minimum from t[i-][j-1], t[i-1][j],t[i][j-1]. return the value at t[n][m]</t>
   </si>
 </sst>
 </file>
@@ -2128,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2160,7 +2160,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2179,7 +2179,7 @@
         <v>465</v>
       </c>
       <c r="D6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21">
@@ -2193,7 +2193,7 @@
         <v>465</v>
       </c>
       <c r="D7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21">
@@ -2207,7 +2207,7 @@
         <v>465</v>
       </c>
       <c r="D8" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21">
@@ -2221,7 +2221,7 @@
         <v>465</v>
       </c>
       <c r="D9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">
@@ -2235,7 +2235,7 @@
         <v>465</v>
       </c>
       <c r="D10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
@@ -2249,7 +2249,7 @@
         <v>465</v>
       </c>
       <c r="D11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21">
@@ -2263,7 +2263,7 @@
         <v>465</v>
       </c>
       <c r="D12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21">
@@ -2277,7 +2277,7 @@
         <v>465</v>
       </c>
       <c r="D13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21">
@@ -2291,7 +2291,7 @@
         <v>465</v>
       </c>
       <c r="D14" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2814,7 +2814,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="21">
+    <row r="65" spans="1:4" ht="21">
       <c r="A65" s="5" t="s">
         <v>53</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="21">
+    <row r="66" spans="1:4" ht="21">
       <c r="A66" s="5" t="s">
         <v>53</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="21">
+    <row r="67" spans="1:4" ht="21">
       <c r="A67" s="5" t="s">
         <v>53</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="21">
+    <row r="68" spans="1:4" ht="21">
       <c r="A68" s="5" t="s">
         <v>53</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="21">
+    <row r="69" spans="1:4" ht="21">
       <c r="A69" s="5" t="s">
         <v>53</v>
       </c>
@@ -2866,10 +2866,13 @@
         <v>67</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+      <c r="D69" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="21">
       <c r="A70" s="5" t="s">
         <v>53</v>
       </c>
@@ -2880,7 +2883,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="21">
+    <row r="71" spans="1:4" ht="21">
       <c r="A71" s="5" t="s">
         <v>53</v>
       </c>
@@ -2891,7 +2894,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="21">
+    <row r="72" spans="1:4" ht="21">
       <c r="A72" s="5" t="s">
         <v>53</v>
       </c>
@@ -2899,10 +2902,10 @@
         <v>70</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="21">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="21">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -2913,7 +2916,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="21">
+    <row r="74" spans="1:4" ht="21">
       <c r="A74" s="5" t="s">
         <v>53</v>
       </c>
@@ -2924,7 +2927,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="21">
+    <row r="75" spans="1:4" ht="21">
       <c r="A75" s="5" t="s">
         <v>53</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="21">
+    <row r="76" spans="1:4" ht="21">
       <c r="A76" s="5" t="s">
         <v>53</v>
       </c>
@@ -2946,7 +2949,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="21">
+    <row r="77" spans="1:4" ht="21">
       <c r="A77" s="5" t="s">
         <v>53</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="21">
+    <row r="78" spans="1:4" ht="21">
       <c r="A78" s="5" t="s">
         <v>53</v>
       </c>
@@ -2968,7 +2971,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="21">
+    <row r="79" spans="1:4" ht="21">
       <c r="A79" s="5" t="s">
         <v>53</v>
       </c>
@@ -2979,7 +2982,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="21">
+    <row r="80" spans="1:4" ht="21">
       <c r="A80" s="5" t="s">
         <v>53</v>
       </c>
@@ -3144,7 +3147,7 @@
         <v>465</v>
       </c>
       <c r="D94" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="21">
@@ -3413,7 +3416,7 @@
         <v>117</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="21">
@@ -3490,7 +3493,7 @@
         <v>124</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="21">
@@ -5471,7 +5474,7 @@
         <v>465</v>
       </c>
       <c r="D315" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="21">
@@ -5507,7 +5510,7 @@
         <v>465</v>
       </c>
       <c r="D318" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="21">
@@ -5988,7 +5991,7 @@
         <v>465</v>
       </c>
       <c r="D364" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="21">
@@ -6002,7 +6005,7 @@
         <v>465</v>
       </c>
       <c r="D365" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="21">
@@ -6016,7 +6019,7 @@
         <v>465</v>
       </c>
       <c r="D366" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="367" spans="1:4" ht="21">
@@ -6030,7 +6033,7 @@
         <v>465</v>
       </c>
       <c r="D367" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="21">
@@ -6044,7 +6047,7 @@
         <v>465</v>
       </c>
       <c r="D368" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="369" spans="1:29" ht="21">
@@ -6058,7 +6061,7 @@
         <v>465</v>
       </c>
       <c r="D369" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="370" spans="1:29" ht="21">
@@ -6072,7 +6075,7 @@
         <v>465</v>
       </c>
       <c r="D370" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="371" spans="1:29" ht="21">
@@ -6086,7 +6089,7 @@
         <v>465</v>
       </c>
       <c r="D371" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="372" spans="1:29" ht="21">
@@ -6122,7 +6125,7 @@
         <v>465</v>
       </c>
       <c r="D374" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="375" spans="1:29" ht="21">
@@ -6136,7 +6139,7 @@
         <v>465</v>
       </c>
       <c r="D375" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="376" spans="1:29" ht="21">
@@ -6150,7 +6153,7 @@
         <v>465</v>
       </c>
       <c r="D376" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="377" spans="1:29" ht="21">
@@ -6164,7 +6167,7 @@
         <v>465</v>
       </c>
       <c r="D377" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="378" spans="1:29" ht="21">
@@ -6200,10 +6203,10 @@
         <v>465</v>
       </c>
       <c r="D380" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AC380" s="12" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="381" spans="1:29" ht="21">
@@ -6217,7 +6220,7 @@
         <v>465</v>
       </c>
       <c r="D381" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="382" spans="1:29" ht="21">
@@ -6242,7 +6245,7 @@
         <v>465</v>
       </c>
       <c r="D383" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="384" spans="1:29" ht="21">
@@ -6256,7 +6259,7 @@
         <v>465</v>
       </c>
       <c r="D384" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="385" spans="1:32" ht="21">
@@ -6270,7 +6273,7 @@
         <v>465</v>
       </c>
       <c r="D385" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="386" spans="1:32" ht="21">
@@ -6284,10 +6287,10 @@
         <v>465</v>
       </c>
       <c r="D386" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AF386" s="12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="387" spans="1:32" ht="21">
@@ -6301,7 +6304,7 @@
         <v>465</v>
       </c>
       <c r="D387" s="12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="388" spans="1:32" ht="21">
@@ -6315,7 +6318,7 @@
         <v>465</v>
       </c>
       <c r="D388" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="389" spans="1:32" ht="21">
@@ -6329,7 +6332,7 @@
         <v>465</v>
       </c>
       <c r="D389" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="390" spans="1:32" ht="21">
@@ -6343,7 +6346,7 @@
         <v>465</v>
       </c>
       <c r="D390" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="391" spans="1:32" ht="21">
@@ -6357,7 +6360,7 @@
         <v>465</v>
       </c>
       <c r="D391" s="12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="392" spans="1:32" ht="21">
@@ -6371,7 +6374,7 @@
         <v>465</v>
       </c>
       <c r="D392" s="12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="393" spans="1:32" ht="21">
@@ -6385,7 +6388,7 @@
         <v>465</v>
       </c>
       <c r="D393" s="12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="394" spans="1:32" ht="21">
@@ -6552,7 +6555,7 @@
         <v>465</v>
       </c>
       <c r="D410" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="411" spans="1:5" ht="21">
@@ -6566,10 +6569,10 @@
         <v>465</v>
       </c>
       <c r="D411" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E411" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="412" spans="1:5" ht="21">
@@ -6583,7 +6586,7 @@
         <v>465</v>
       </c>
       <c r="D412" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="413" spans="1:5" ht="21">
@@ -6597,7 +6600,7 @@
         <v>465</v>
       </c>
       <c r="D413" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="414" spans="1:5" ht="21">
@@ -6611,7 +6614,7 @@
         <v>465</v>
       </c>
       <c r="D414" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="415" spans="1:5" ht="21">
@@ -6625,7 +6628,7 @@
         <v>465</v>
       </c>
       <c r="D415" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="416" spans="1:5" ht="21">
@@ -6639,7 +6642,7 @@
         <v>465</v>
       </c>
       <c r="D416" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="417" spans="1:66" ht="21">
@@ -6653,7 +6656,7 @@
         <v>465</v>
       </c>
       <c r="D417" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="418" spans="1:66" ht="21">
@@ -6667,7 +6670,7 @@
         <v>465</v>
       </c>
       <c r="D418" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="419" spans="1:66" ht="21">
@@ -6681,7 +6684,7 @@
         <v>465</v>
       </c>
       <c r="D419" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="420" spans="1:66" ht="21">
@@ -6706,7 +6709,7 @@
         <v>465</v>
       </c>
       <c r="D421" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="422" spans="1:66" ht="21">
@@ -6720,7 +6723,7 @@
         <v>465</v>
       </c>
       <c r="D422" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="423" spans="1:66" ht="21">
@@ -6734,7 +6737,7 @@
         <v>465</v>
       </c>
       <c r="D423" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="424" spans="1:66" ht="21">
@@ -6748,7 +6751,7 @@
         <v>465</v>
       </c>
       <c r="D424" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="425" spans="1:66" ht="21">
@@ -6784,7 +6787,7 @@
         <v>465</v>
       </c>
       <c r="D427" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="428" spans="1:66" ht="21">
@@ -6798,7 +6801,7 @@
         <v>465</v>
       </c>
       <c r="D428" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="429" spans="1:66" ht="21">
@@ -6845,10 +6848,10 @@
         <v>465</v>
       </c>
       <c r="D432" t="s">
+        <v>518</v>
+      </c>
+      <c r="BN432" t="s">
         <v>519</v>
-      </c>
-      <c r="BN432" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="433" spans="1:4" ht="21">
@@ -6950,7 +6953,7 @@
         <v>465</v>
       </c>
       <c r="D441" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="442" spans="1:4" ht="21">
@@ -6964,7 +6967,7 @@
         <v>465</v>
       </c>
       <c r="D442" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="443" spans="1:4" ht="21">
@@ -6989,7 +6992,7 @@
         <v>465</v>
       </c>
       <c r="D444" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="445" spans="1:4" ht="21">
@@ -7003,7 +7006,7 @@
         <v>465</v>
       </c>
       <c r="D445" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="446" spans="1:4" ht="21">
@@ -7061,7 +7064,7 @@
         <v>465</v>
       </c>
       <c r="D450" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="451" spans="1:4" ht="21">
@@ -7174,7 +7177,7 @@
         <v>465</v>
       </c>
       <c r="D460" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="461" spans="1:4" ht="21">
@@ -7210,7 +7213,7 @@
         <v>465</v>
       </c>
       <c r="D463" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="464" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added  Longest repeating subsequence
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F48931-C90D-4388-AD04-394CF04F419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7103EE5B-FF8F-4BCC-BB0D-FDF29EADBABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9024" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="538">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1665,6 +1665,9 @@
   </si>
   <si>
     <t>Done with DP: int the matrix with n+1 and m+1 where n and m are the length of s and t respectively. Now init the value at t[0][0] as 0 because both strings are equal. Now from i=0 to n+1, place t[i][0] = I and for j=0 to m+1 place t[0][j]=j. Now traverslse the matrix from 1 to n+1 and for j= 1 to m+1. For any point where s[i-1]==t[j-1], take the diagonally previous element at t[i-1][j-1] and place in t[i][j] else take minimum from t[i-][j-1], t[i-1][j],t[i][j-1]. return the value at t[n][m]</t>
+  </si>
+  <si>
+    <t>DP was applied: Simply run LCS for the same string but add the condition for checking if i!=j, then only 1+ t[i-1[j-1]. Otherwise take max of t[i-1][j] and t[i][j-1]</t>
   </si>
 </sst>
 </file>
@@ -2128,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2655,7 +2658,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21">
+    <row r="49" spans="1:4" ht="21">
       <c r="A49" s="8" t="s">
         <v>42</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21">
+    <row r="50" spans="1:4" ht="21">
       <c r="A50" s="8" t="s">
         <v>42</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21">
+    <row r="51" spans="1:4" ht="21">
       <c r="A51" s="8" t="s">
         <v>42</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21">
+    <row r="52" spans="1:4" ht="21">
       <c r="A52" s="8" t="s">
         <v>42</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21">
+    <row r="53" spans="1:4" ht="21">
       <c r="A53" s="8" t="s">
         <v>42</v>
       </c>
@@ -2710,12 +2713,12 @@
         <v>466</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21">
+    <row r="55" spans="1:4" ht="21">
       <c r="A55" s="5"/>
       <c r="B55" s="7"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="21">
+    <row r="56" spans="1:4" ht="21">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -2726,7 +2729,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="21">
+    <row r="57" spans="1:4" ht="21">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21">
+    <row r="58" spans="1:4" ht="21">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
@@ -2748,7 +2751,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="21">
+    <row r="59" spans="1:4" ht="21">
       <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21">
+    <row r="60" spans="1:4" ht="21">
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
@@ -2770,7 +2773,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="21">
+    <row r="61" spans="1:4" ht="21">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="21">
+    <row r="62" spans="1:4" ht="21">
       <c r="A62" s="5" t="s">
         <v>53</v>
       </c>
@@ -2792,7 +2795,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="21">
+    <row r="63" spans="1:4" ht="21">
       <c r="A63" s="5" t="s">
         <v>53</v>
       </c>
@@ -2803,7 +2806,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21">
+    <row r="64" spans="1:4" ht="21">
       <c r="A64" s="5" t="s">
         <v>53</v>
       </c>
@@ -2811,7 +2814,10 @@
         <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
+      </c>
+      <c r="D64" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added explanation and revision of minJUmps
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7103EE5B-FF8F-4BCC-BB0D-FDF29EADBABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1F7256-318D-4CC5-97EE-F0FA97AB56A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9024" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="539">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1668,6 +1668,9 @@
   </si>
   <si>
     <t>DP was applied: Simply run LCS for the same string but add the condition for checking if i!=j, then only 1+ t[i-1[j-1]. Otherwise take max of t[i-1][j] and t[i][j-1]</t>
+  </si>
+  <si>
+    <t>keep a track of the maximum reach you can go from any point in the array, this can be done with current index+value of array at index, take max of this element while iteration, at any point steps become 0, take the counter for steps up by one point. replace the reamaing steps varibale with maxReach - currentIndex (becuase you have come ahead a bit). If the maxReach is less than or equal to the current index that means you are stuck in a 0 and it is impossible to traverse the array. Thus return -1. init the first number of steps available as arr[0] and startrr the jump counter from 1 as you have to take the first jump no matter what.</t>
   </si>
 </sst>
 </file>
@@ -2131,18 +2134,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2306,6 +2309,9 @@
       </c>
       <c r="C15" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D15" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added constant space to find duplicate number
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1F7256-318D-4CC5-97EE-F0FA97AB56A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E43DA7-C5F5-4D08-B8A6-98885296CC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="540">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1671,6 +1671,9 @@
   </si>
   <si>
     <t>keep a track of the maximum reach you can go from any point in the array, this can be done with current index+value of array at index, take max of this element while iteration, at any point steps become 0, take the counter for steps up by one point. replace the reamaing steps varibale with maxReach - currentIndex (becuase you have come ahead a bit). If the maxReach is less than or equal to the current index that means you are stuck in a 0 and it is impossible to traverse the array. Thus return -1. init the first number of steps available as arr[0] and startrr the jump counter from 1 as you have to take the first jump no matter what.</t>
+  </si>
+  <si>
+    <t>Easy way to do this will be to simply sort the array and check if any adjacent elements are same. If you wanna do it in linear time and in constant space, you have to use fast and slow algo from linked list. This can be done by initializing two pointers, slow and fast where slow is arr[0] and fast is arr[arr[0]] this way if there is ever a repeating element slow ==fast. run a while loop till you find slow==fast. Each iteration will have slow = nums[slow] and fast = nums[nums[fast]] . Once while ends, reinitialize fast to 0 and  make slow = nums[slow] and fast = nums[fast]. once this loop ends return slow</t>
   </si>
 </sst>
 </file>
@@ -2135,7 +2138,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2323,6 +2326,9 @@
       </c>
       <c r="C16" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D16" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added choclate dist explanation
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498863CF-6219-4D93-B3D8-616A0344B9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9E59CE-BFD1-447E-8399-CFCE0057A5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="541">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1674,6 +1674,9 @@
   </si>
   <si>
     <t>Easy way to do this will be to simply sort the array and check if any adjacent elements are same. If you wanna do it in linear time and in constant space, you have to use fast and slow algo from linked list. This can be done by initializing two pointers, slow and fast where slow is arr[0] and fast is arr[arr[0]] this way if there is ever a repeating element slow ==fast. run a while loop till you find slow==fast. Each iteration will have slow = nums[slow] and fast = nums[nums[fast]] . Once while ends, reinitialize fast to 0 and  make slow = nums[slow] and fast = nums[fast]. once this loop ends return slow</t>
+  </si>
+  <si>
+    <t>Init a start at zero and make a new variable for keeping the minimum value. Sort the array, now traverse the array with start incremeneting till start+m-1&lt;n. Find min between the variable for minimum and the current difference between the start+m and start. return the variable in the end.</t>
   </si>
 </sst>
 </file>
@@ -2137,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2507,7 +2510,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21">
+    <row r="33" spans="1:4" ht="21">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21">
+    <row r="34" spans="1:4" ht="21">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21">
+    <row r="35" spans="1:4" ht="21">
       <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
@@ -2539,8 +2542,11 @@
       <c r="C35" s="4" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="21">
+      <c r="D35" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="21">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21">
+    <row r="37" spans="1:4" ht="21">
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
@@ -2562,7 +2568,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21">
+    <row r="38" spans="1:4" ht="21">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
@@ -2573,7 +2579,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21">
+    <row r="39" spans="1:4" ht="21">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21">
+    <row r="40" spans="1:4" ht="21">
       <c r="A40" s="5" t="s">
         <v>5</v>
       </c>
@@ -2595,7 +2601,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21">
+    <row r="41" spans="1:4" ht="21">
       <c r="A41" s="5" t="s">
         <v>5</v>
       </c>
@@ -2606,16 +2612,16 @@
         <v>465</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21">
+    <row r="42" spans="1:4" ht="21">
       <c r="B42" s="7"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" ht="21">
+    <row r="43" spans="1:4" ht="21">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="21">
+    <row r="44" spans="1:4" ht="21">
       <c r="A44" s="8" t="s">
         <v>42</v>
       </c>
@@ -2626,7 +2632,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21">
+    <row r="45" spans="1:4" ht="21">
       <c r="A45" s="8" t="s">
         <v>42</v>
       </c>
@@ -2637,7 +2643,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21">
+    <row r="46" spans="1:4" ht="21">
       <c r="A46" s="8" t="s">
         <v>42</v>
       </c>
@@ -2648,7 +2654,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21">
+    <row r="47" spans="1:4" ht="21">
       <c r="A47" s="8" t="s">
         <v>42</v>
       </c>
@@ -2659,7 +2665,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21">
+    <row r="48" spans="1:4" ht="21">
       <c r="A48" s="8" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
explanation for merge two array no extra space
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9E59CE-BFD1-447E-8399-CFCE0057A5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5D5133-9FDF-49A4-A021-C0B4CF534F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="542">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1677,6 +1677,9 @@
   </si>
   <si>
     <t>Init a start at zero and make a new variable for keeping the minimum value. Sort the array, now traverse the array with start incremeneting till start+m-1&lt;n. Find min between the variable for minimum and the current difference between the start+m and start. return the variable in the end.</t>
+  </si>
+  <si>
+    <t>Take two pointers for arr1 and one pointer for array 2. init i=0 and k = n-1 for arr1 pointer and j=0 for array two's pointer, now traverse the array and at any point arr1[i]&gt;arr2[j], swap arr2[j] with arr[k] k-- j++ else do i++. At last sort both the arrays</t>
   </si>
 </sst>
 </file>
@@ -2141,7 +2144,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2334,7 +2337,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21">
+    <row r="17" spans="1:4" ht="21">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -2344,8 +2347,11 @@
       <c r="C17" s="4" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="21">
+      <c r="D17" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="21">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -2356,7 +2362,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21">
+    <row r="19" spans="1:4" ht="21">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -2367,7 +2373,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21">
+    <row r="20" spans="1:4" ht="21">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -2378,7 +2384,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21">
+    <row r="21" spans="1:4" ht="21">
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2389,7 +2395,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21">
+    <row r="22" spans="1:4" ht="21">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -2400,7 +2406,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21">
+    <row r="23" spans="1:4" ht="21">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2411,7 +2417,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21">
+    <row r="24" spans="1:4" ht="21">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -2422,7 +2428,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21">
+    <row r="25" spans="1:4" ht="21">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -2433,7 +2439,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21">
+    <row r="26" spans="1:4" ht="21">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21">
+    <row r="27" spans="1:4" ht="21">
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
@@ -2455,7 +2461,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21">
+    <row r="28" spans="1:4" ht="21">
       <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
@@ -2466,7 +2472,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21">
+    <row r="29" spans="1:4" ht="21">
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
@@ -2477,7 +2483,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21">
+    <row r="30" spans="1:4" ht="21">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -2488,7 +2494,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21">
+    <row r="31" spans="1:4" ht="21">
       <c r="A31" s="5" t="s">
         <v>5</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21">
+    <row r="32" spans="1:4" ht="21">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
added explanation in excel
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8D7039-796E-4E67-B525-3714AAE69319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DF120B-348F-4783-8E35-70EACD2FF0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1685,14 +1685,14 @@
     <t>Sort the given meets with the start times of the pairs. Now make a new array to hold the ans and push the first interval inside, loop through the array from 1. If the interval at value i has start time greater than end time of the last element you inserted, inserrt the interval inside the answer vector, else , take the max of the  ending time of the lastt interval added vs end time of the interval at i and place it inside the last element in the answer vector's end time. return ans vector</t>
   </si>
   <si>
-    <t>start from the last element in reverse order, find the first element that is less than the element at right side of it . Set the last index to the element that is greater than element that was found earler. Swap these elements and reverse the vector from index t+1 to end</t>
+    <t>Approch:start from the last element in reverse order, find the first element that is less than the element at right side of it and mark that element as t . Set the last index to the element that is greater than element that was found at t and give it index r. Swap these elements and reverse the vector from index t+1 to end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1763,6 +1763,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF5C6370"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1785,7 +1791,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1811,6 +1817,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2150,7 +2159,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2395,7 +2404,7 @@
       <c r="C20" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="13" t="s">
         <v>543</v>
       </c>
     </row>

</xml_diff>

<commit_message>
addeed explanation of stock price buying
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E871C2-5632-4DD1-911B-63A7D2F11ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54DCCDA-1B44-4595-ABD5-1B26F84A8268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="546">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1689,6 +1689,9 @@
   </si>
   <si>
     <t>Follows merge sort, split the array from the middle recursively and them merge those parts such a way that the value witht the lesser value comes first, how ever at any point the value at left side is more than value at right side increse the count of inversions. inversion= inversion+(mid-i)</t>
+  </si>
+  <si>
+    <t>Loop through the array of prices, find the minimum price of the stock at each iteration. If the current value is more than buy value which is the min so far, then maximise  the difference between the current iteration in prices and the price you bought at,</t>
   </si>
 </sst>
 </file>
@@ -2161,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2434,6 +2437,9 @@
       </c>
       <c r="C22" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D22" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added explanaion of pair
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54DCCDA-1B44-4595-ABD5-1B26F84A8268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C22988F-5ABE-41AB-8BB2-D64C93C86FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="547">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1692,6 +1692,9 @@
   </si>
   <si>
     <t>Loop through the array of prices, find the minimum price of the stock at each iteration. If the current value is more than buy value which is the min so far, then maximise  the difference between the current iteration in prices and the price you bought at,</t>
+  </si>
+  <si>
+    <t>Make a map to count the  frequency of the array element, now loop through the array again with a variable count, where count+=map[k-arr[i]] . If the arr[i]==k-arr[i], then decrement count by 1. finally reaturn count/2</t>
   </si>
 </sst>
 </file>
@@ -2164,8 +2167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -2451,6 +2454,9 @@
       </c>
       <c r="C23" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D23" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21">

</xml_diff>

<commit_message>
updated common elements in three array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C22988F-5ABE-41AB-8BB2-D64C93C86FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27B60CB-2162-49A1-A286-2A20D84F3426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="547">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>

</xml_diff>

<commit_message>
explnation for max product subarray
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03BB6A4-885A-4546-BB0D-524AE128F734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBE3CCB-94CA-4C06-A934-129C5901AAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="1440" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="552">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1707,6 +1707,9 @@
   </si>
   <si>
     <t>Tricky: You have to make an array that contains the digits of the answer, for this make an array with max size. Now init a array size with 1; loop from 2 to given number N. for each iteration multiply each digit inside of the array till size with the iteration int i. Make sure it is only on digits place and increase tthe size whenever there is a carry after the loop. Once done, copy the result in reverse order from arrray size to 0 in another array and return this array</t>
+  </si>
+  <si>
+    <t>make two varibales left and right and make them both 1. Now run a for loop for the given array, if l==0, then make l = arr[i]. Else l=l*arr[i]. Same with r but instead of i use n-i-1 as it is coming from behind. This will make sure to take care of any product going at zero and reset it from current value. Take make of l and r at each iteration.</t>
   </si>
 </sst>
 </file>
@@ -2179,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2536,6 +2539,9 @@
       </c>
       <c r="C28" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D28" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added explanation of longestConsecutiveSubSeq
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBE3CCB-94CA-4C06-A934-129C5901AAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB57B1CB-08A6-434C-8593-77015665B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="1440" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="553">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1710,6 +1710,9 @@
   </si>
   <si>
     <t>make two varibales left and right and make them both 1. Now run a for loop for the given array, if l==0, then make l = arr[i]. Else l=l*arr[i]. Same with r but instead of i use n-i-1 as it is coming from behind. This will make sure to take care of any product going at zero and reset it from current value. Take make of l and r at each iteration.</t>
+  </si>
+  <si>
+    <t>Make a set of all the numbers, now loop through the set and keep elelement a as iterator. If set contains s-1, continue else count till s contains s+1, make this a new variable, y = x+1, and while(set contains y) y++;. Once the while ends, take max of current ans and y-a, return max</t>
   </si>
 </sst>
 </file>
@@ -2182,8 +2185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:BN481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2553,6 +2556,9 @@
       </c>
       <c r="C29" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D29" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="21">

</xml_diff>

<commit_message>
find elements that apprear more than n/k times
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB57B1CB-08A6-434C-8593-77015665B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08678C1-B768-4DDF-814C-88F42C896A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="1440" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="554">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1713,6 +1713,9 @@
   </si>
   <si>
     <t>Make a set of all the numbers, now loop through the set and keep elelement a as iterator. If set contains s-1, continue else count till s contains s+1, make this a new variable, y = x+1, and while(set contains y) y++;. Once the while ends, take max of current ans and y-a, return max</t>
+  </si>
+  <si>
+    <t>If you have no space constrains simply make an unordered map and count the number of times any element occurs, the mloop through the map and see whichelements are appreaing more times then the condition provided.</t>
   </si>
 </sst>
 </file>
@@ -2186,7 +2189,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2570,6 +2573,9 @@
       </c>
       <c r="C30" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D30" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="21">

</xml_diff>

<commit_message>
stocks at 2 transaction solution added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08678C1-B768-4DDF-814C-88F42C896A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB8E61-89BD-45E3-B9A6-D93068E7BC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="1440" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="19920" yWindow="1425" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="555">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1716,6 +1716,9 @@
   </si>
   <si>
     <t>If you have no space constrains simply make an unordered map and count the number of times any element occurs, the mloop through the map and see whichelements are appreaing more times then the condition provided.</t>
+  </si>
+  <si>
+    <t>Make an array for profits, loop backwards in the prices array and find the max prices and max profit you can make, now loop from left to right on prices and find the min prices, along with this put the max between profit so far vs profit at i + price at i - min_price, return the last element of the profit array for your ans</t>
   </si>
 </sst>
 </file>
@@ -2189,7 +2192,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2587,6 +2590,9 @@
       </c>
       <c r="C31" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D31" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added explanation for three sum
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB8E61-89BD-45E3-B9A6-D93068E7BC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074A9B3D-BA3E-4C52-BB34-780E01C7141F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19920" yWindow="1425" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="557">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1719,6 +1719,12 @@
   </si>
   <si>
     <t>Make an array for profits, loop backwards in the prices array and find the max prices and max profit you can make, now loop from left to right on prices and find the min prices, along with this put the max between profit so far vs profit at i + price at i - min_price, return the last element of the profit array for your ans</t>
+  </si>
+  <si>
+    <t>Make a set from the second array and traverse the first, if any element is found remove it from the set. IF the size of the set is 0  at the end, return YES or return false</t>
+  </si>
+  <si>
+    <t>Sort the given array, then loop through from i= 0 to n-2, if i&gt;0 and arr[i]==arr[i-1] continue because you have already evaluated the given duplicate in the last case. Now for each I, if arr[i]+arr[i+1] + arr[i+2} exceeds the given target then you won't be able to find the targer and break the loop. If arr[i]+arr[n-1]+arr[n-2] is less than target then continue to the next loop. THne make two pointers left and right and find the sum of ar[i] + a[left]+ar[right]. IF the sum is equal to target return true, if sum exceed, right-- if the sum is less make left++. If loop ends return false</t>
   </si>
 </sst>
 </file>
@@ -2192,7 +2198,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2605,6 +2611,9 @@
       <c r="C32" s="4" t="s">
         <v>465</v>
       </c>
+      <c r="D32" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="21">
       <c r="A33" s="5" t="s">
@@ -2615,6 +2624,9 @@
       </c>
       <c r="C33" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D33" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="21">

</xml_diff>

<commit_message>
added explanation for three way partition
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\CPP\450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148AAE26-9BD5-409A-849F-0BB8B423CAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8098635-7DDF-434B-9F01-98DC4A986B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48825" yWindow="2640" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="17505" yWindow="960" windowWidth="28800" windowHeight="11385" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="560">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1731,6 +1731,9 @@
   </si>
   <si>
     <t>Iterate throught the array till the sum of elements so far is less than or equal to the target, the momnet it becomes greater than the target start substracting the element in addition from the least. Count the number of element and return the minimum at which the sum was greater.</t>
+  </si>
+  <si>
+    <t>Make 3 sets for each condition and then empty them placing the values in the original vector.</t>
   </si>
 </sst>
 </file>
@@ -2204,7 +2207,7 @@
   <dimension ref="A1:BN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2686,6 +2689,9 @@
       </c>
       <c r="C37" s="4" t="s">
         <v>465</v>
+      </c>
+      <c r="D37" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="21">

</xml_diff>